<commit_message>
Added CRYP to ExternalPurpose1Code
Added CRYP to ExternalPurpose1Code
</commit_message>
<xml_diff>
--- a/ISO_External_Codeset.xlsx
+++ b/ISO_External_Codeset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/OpenBanking/GitHub/External_Internal_CodeSets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/GitHub-repos/External_Internal_CodeSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9567958B-0CA4-9D41-8DB3-949BC192AFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57DBED4-A0DE-CB4E-BA5B-16FFB35A5901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19820" xr2:uid="{FBBA5019-91DA-4C4F-B9CD-8AE24E623AAD}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19820" xr2:uid="{FBBA5019-91DA-4C4F-B9CD-8AE24E623AAD}"/>
   </bookViews>
   <sheets>
     <sheet name="ISO_External_Codeset" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="1927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2926" uniqueCount="1930">
   <si>
     <t>Code Set</t>
   </si>
@@ -5844,6 +5844,15 @@
   </si>
   <si>
     <t>Tax accessed by state jurisdications within a country.</t>
+  </si>
+  <si>
+    <t>CRYP</t>
+  </si>
+  <si>
+    <t>CryptoTransaction</t>
+  </si>
+  <si>
+    <t>Transaction is for the purchase of cryptocurrency</t>
   </si>
 </sst>
 </file>
@@ -6395,8 +6404,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{29E1F7B0-255A-A04F-A5BA-2B2FDA1E8B0D}" name="Table1" displayName="Table1" ref="A1:E692" totalsRowShown="0">
-  <autoFilter ref="A1:E692" xr:uid="{29E1F7B0-255A-A04F-A5BA-2B2FDA1E8B0D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{29E1F7B0-255A-A04F-A5BA-2B2FDA1E8B0D}" name="Table1" displayName="Table1" ref="A1:E693" totalsRowShown="0">
+  <autoFilter ref="A1:E693" xr:uid="{29E1F7B0-255A-A04F-A5BA-2B2FDA1E8B0D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{568DECC5-0A29-0D4B-8F34-A37284783E08}" name="Code Set"/>
     <tableColumn id="2" xr3:uid="{7C2DD376-A83D-244C-9FF9-52150D88C761}" name="Code Value"/>
@@ -6725,10 +6734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1898038C-F655-9844-A304-6CA45952208C}">
-  <dimension ref="A1:E692"/>
+  <dimension ref="A1:E693"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A589" workbookViewId="0">
+      <selection activeCell="D613" sqref="D613"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15784,32 +15793,32 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="614" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A614" t="s">
-        <v>1745</v>
+        <v>850</v>
       </c>
       <c r="B614" t="s">
-        <v>36</v>
+        <v>1927</v>
       </c>
       <c r="C614" t="s">
-        <v>37</v>
+        <v>1928</v>
       </c>
       <c r="D614" s="1" t="s">
-        <v>1746</v>
-      </c>
-    </row>
-    <row r="615" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="615" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A615" t="s">
         <v>1745</v>
       </c>
       <c r="B615" t="s">
-        <v>1747</v>
+        <v>36</v>
       </c>
       <c r="C615" t="s">
-        <v>1748</v>
+        <v>37</v>
       </c>
       <c r="D615" s="1" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="616" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15817,13 +15826,13 @@
         <v>1745</v>
       </c>
       <c r="B616" t="s">
-        <v>1750</v>
+        <v>1747</v>
       </c>
       <c r="C616" t="s">
-        <v>1751</v>
+        <v>1748</v>
       </c>
       <c r="D616" s="1" t="s">
-        <v>1752</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="617" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15831,55 +15840,55 @@
         <v>1745</v>
       </c>
       <c r="B617" t="s">
-        <v>1753</v>
+        <v>1750</v>
       </c>
       <c r="C617" t="s">
-        <v>1754</v>
+        <v>1751</v>
       </c>
       <c r="D617" s="1" t="s">
-        <v>1755</v>
-      </c>
-    </row>
-    <row r="618" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="618" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A618" t="s">
         <v>1745</v>
       </c>
       <c r="B618" t="s">
-        <v>42</v>
+        <v>1753</v>
       </c>
       <c r="C618" t="s">
-        <v>43</v>
+        <v>1754</v>
       </c>
       <c r="D618" s="1" t="s">
-        <v>1756</v>
-      </c>
-    </row>
-    <row r="619" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="619" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A619" t="s">
         <v>1745</v>
       </c>
       <c r="B619" t="s">
-        <v>1757</v>
+        <v>42</v>
       </c>
       <c r="C619" t="s">
-        <v>1758</v>
+        <v>43</v>
       </c>
       <c r="D619" s="1" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="620" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="620" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A620" t="s">
         <v>1745</v>
       </c>
       <c r="B620" t="s">
-        <v>549</v>
+        <v>1757</v>
       </c>
       <c r="C620" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="D620" s="1" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="621" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15887,13 +15896,13 @@
         <v>1745</v>
       </c>
       <c r="B621" t="s">
-        <v>1762</v>
+        <v>549</v>
       </c>
       <c r="C621" t="s">
-        <v>1763</v>
+        <v>1760</v>
       </c>
       <c r="D621" s="1" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="622" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15901,13 +15910,13 @@
         <v>1745</v>
       </c>
       <c r="B622" t="s">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="C622" t="s">
-        <v>1766</v>
+        <v>1763</v>
       </c>
       <c r="D622" s="1" t="s">
-        <v>1767</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="623" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15915,41 +15924,41 @@
         <v>1745</v>
       </c>
       <c r="B623" t="s">
-        <v>1768</v>
+        <v>1765</v>
       </c>
       <c r="C623" t="s">
-        <v>1769</v>
+        <v>1766</v>
       </c>
       <c r="D623" s="1" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="624" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="624" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A624" t="s">
         <v>1745</v>
       </c>
       <c r="B624" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="C624" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
       <c r="D624" s="1" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="625" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A625" t="s">
         <v>1745</v>
       </c>
       <c r="B625" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
       <c r="C625" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="D625" s="1" t="s">
-        <v>1776</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="626" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15957,13 +15966,13 @@
         <v>1745</v>
       </c>
       <c r="B626" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
       <c r="C626" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
       <c r="D626" s="1" t="s">
-        <v>1779</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="627" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15971,13 +15980,13 @@
         <v>1745</v>
       </c>
       <c r="B627" t="s">
-        <v>1780</v>
+        <v>1777</v>
       </c>
       <c r="C627" t="s">
-        <v>1781</v>
+        <v>1778</v>
       </c>
       <c r="D627" s="1" t="s">
-        <v>1782</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="628" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15985,13 +15994,13 @@
         <v>1745</v>
       </c>
       <c r="B628" t="s">
-        <v>1783</v>
+        <v>1780</v>
       </c>
       <c r="C628" t="s">
-        <v>1784</v>
+        <v>1781</v>
       </c>
       <c r="D628" s="1" t="s">
-        <v>1785</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="629" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15999,13 +16008,13 @@
         <v>1745</v>
       </c>
       <c r="B629" t="s">
-        <v>1786</v>
+        <v>1783</v>
       </c>
       <c r="C629" t="s">
-        <v>1787</v>
+        <v>1784</v>
       </c>
       <c r="D629" s="1" t="s">
-        <v>1788</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="630" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16013,13 +16022,13 @@
         <v>1745</v>
       </c>
       <c r="B630" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="C630" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="D630" s="1" t="s">
-        <v>1791</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="631" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16027,13 +16036,13 @@
         <v>1745</v>
       </c>
       <c r="B631" t="s">
-        <v>773</v>
+        <v>1789</v>
       </c>
       <c r="C631" t="s">
-        <v>1792</v>
+        <v>1790</v>
       </c>
       <c r="D631" s="1" t="s">
-        <v>1793</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="632" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16041,13 +16050,13 @@
         <v>1745</v>
       </c>
       <c r="B632" t="s">
-        <v>1794</v>
+        <v>773</v>
       </c>
       <c r="C632" t="s">
-        <v>1795</v>
+        <v>1792</v>
       </c>
       <c r="D632" s="1" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="633" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16055,13 +16064,13 @@
         <v>1745</v>
       </c>
       <c r="B633" t="s">
-        <v>48</v>
+        <v>1794</v>
       </c>
       <c r="C633" t="s">
-        <v>49</v>
+        <v>1795</v>
       </c>
       <c r="D633" s="1" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="634" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16069,13 +16078,13 @@
         <v>1745</v>
       </c>
       <c r="B634" t="s">
-        <v>1798</v>
+        <v>48</v>
       </c>
       <c r="C634" t="s">
-        <v>1799</v>
+        <v>49</v>
       </c>
       <c r="D634" s="1" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="635" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16083,13 +16092,13 @@
         <v>1745</v>
       </c>
       <c r="B635" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
       <c r="C635" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
       <c r="D635" s="1" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="636" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16097,13 +16106,13 @@
         <v>1745</v>
       </c>
       <c r="B636" t="s">
-        <v>1804</v>
+        <v>1801</v>
       </c>
       <c r="C636" t="s">
-        <v>1805</v>
+        <v>1802</v>
       </c>
       <c r="D636" s="1" t="s">
-        <v>1806</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="637" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16111,13 +16120,13 @@
         <v>1745</v>
       </c>
       <c r="B637" t="s">
-        <v>1807</v>
+        <v>1804</v>
       </c>
       <c r="C637" t="s">
-        <v>1808</v>
+        <v>1805</v>
       </c>
       <c r="D637" s="1" t="s">
-        <v>1809</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="638" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16125,13 +16134,13 @@
         <v>1745</v>
       </c>
       <c r="B638" t="s">
-        <v>51</v>
+        <v>1807</v>
       </c>
       <c r="C638" t="s">
-        <v>52</v>
+        <v>1808</v>
       </c>
       <c r="D638" s="1" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="639" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16139,13 +16148,13 @@
         <v>1745</v>
       </c>
       <c r="B639" t="s">
-        <v>1811</v>
+        <v>51</v>
       </c>
       <c r="C639" t="s">
-        <v>1812</v>
+        <v>52</v>
       </c>
       <c r="D639" s="1" t="s">
-        <v>1813</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="640" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16153,13 +16162,13 @@
         <v>1745</v>
       </c>
       <c r="B640" t="s">
-        <v>1814</v>
+        <v>1811</v>
       </c>
       <c r="C640" t="s">
-        <v>1815</v>
+        <v>1812</v>
       </c>
       <c r="D640" s="1" t="s">
-        <v>1816</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="641" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16167,13 +16176,13 @@
         <v>1745</v>
       </c>
       <c r="B641" t="s">
-        <v>54</v>
+        <v>1814</v>
       </c>
       <c r="C641" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
       <c r="D641" s="1" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="642" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16181,13 +16190,13 @@
         <v>1745</v>
       </c>
       <c r="B642" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C642" t="s">
-        <v>1819</v>
+        <v>1817</v>
       </c>
       <c r="D642" s="1" t="s">
-        <v>59</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="643" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16195,13 +16204,13 @@
         <v>1745</v>
       </c>
       <c r="B643" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C643" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="D643" s="1" t="s">
-        <v>1821</v>
+        <v>59</v>
       </c>
     </row>
     <row r="644" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16209,13 +16218,13 @@
         <v>1745</v>
       </c>
       <c r="B644" t="s">
-        <v>1822</v>
+        <v>60</v>
       </c>
       <c r="C644" t="s">
-        <v>1823</v>
+        <v>1820</v>
       </c>
       <c r="D644" s="1" t="s">
-        <v>1824</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="645" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16223,13 +16232,13 @@
         <v>1745</v>
       </c>
       <c r="B645" t="s">
-        <v>63</v>
+        <v>1822</v>
       </c>
       <c r="C645" t="s">
-        <v>64</v>
+        <v>1823</v>
       </c>
       <c r="D645" s="1" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="646" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16237,41 +16246,41 @@
         <v>1745</v>
       </c>
       <c r="B646" t="s">
-        <v>1826</v>
+        <v>63</v>
       </c>
       <c r="C646" t="s">
-        <v>1827</v>
+        <v>64</v>
       </c>
       <c r="D646" s="1" t="s">
-        <v>1828</v>
-      </c>
-    </row>
-    <row r="647" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="647" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A647" t="s">
         <v>1745</v>
       </c>
       <c r="B647" t="s">
-        <v>66</v>
+        <v>1826</v>
       </c>
       <c r="C647" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
       <c r="D647" s="1" t="s">
-        <v>1830</v>
-      </c>
-    </row>
-    <row r="648" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="648" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A648" t="s">
         <v>1745</v>
       </c>
       <c r="B648" t="s">
-        <v>1831</v>
+        <v>66</v>
       </c>
       <c r="C648" t="s">
-        <v>1832</v>
+        <v>1829</v>
       </c>
       <c r="D648" s="1" t="s">
-        <v>1833</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="649" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16279,13 +16288,13 @@
         <v>1745</v>
       </c>
       <c r="B649" t="s">
-        <v>1834</v>
+        <v>1831</v>
       </c>
       <c r="C649" t="s">
-        <v>1835</v>
+        <v>1832</v>
       </c>
       <c r="D649" s="1" t="s">
-        <v>1836</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="650" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16293,13 +16302,13 @@
         <v>1745</v>
       </c>
       <c r="B650" t="s">
-        <v>1837</v>
+        <v>1834</v>
       </c>
       <c r="C650" t="s">
-        <v>1838</v>
+        <v>1835</v>
       </c>
       <c r="D650" s="1" t="s">
-        <v>1839</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="651" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16307,13 +16316,13 @@
         <v>1745</v>
       </c>
       <c r="B651" t="s">
-        <v>72</v>
+        <v>1837</v>
       </c>
       <c r="C651" t="s">
-        <v>73</v>
+        <v>1838</v>
       </c>
       <c r="D651" s="1" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="652" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16321,13 +16330,13 @@
         <v>1745</v>
       </c>
       <c r="B652" t="s">
-        <v>1841</v>
+        <v>72</v>
       </c>
       <c r="C652" t="s">
-        <v>1842</v>
+        <v>73</v>
       </c>
       <c r="D652" s="1" t="s">
-        <v>1843</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="653" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16335,13 +16344,13 @@
         <v>1745</v>
       </c>
       <c r="B653" t="s">
-        <v>1844</v>
+        <v>1841</v>
       </c>
       <c r="C653" t="s">
-        <v>1845</v>
+        <v>1842</v>
       </c>
       <c r="D653" s="1" t="s">
-        <v>1846</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="654" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16349,13 +16358,13 @@
         <v>1745</v>
       </c>
       <c r="B654" t="s">
-        <v>75</v>
+        <v>1844</v>
       </c>
       <c r="C654" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="D654" s="1" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="655" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16363,41 +16372,41 @@
         <v>1745</v>
       </c>
       <c r="B655" t="s">
-        <v>1849</v>
+        <v>75</v>
       </c>
       <c r="C655" t="s">
-        <v>1850</v>
+        <v>1847</v>
       </c>
       <c r="D655" s="1" t="s">
-        <v>1851</v>
-      </c>
-    </row>
-    <row r="656" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A656" t="s">
         <v>1745</v>
       </c>
       <c r="B656" t="s">
-        <v>1852</v>
+        <v>1849</v>
       </c>
       <c r="C656" t="s">
-        <v>1853</v>
+        <v>1850</v>
       </c>
       <c r="D656" s="1" t="s">
-        <v>1854</v>
-      </c>
-    </row>
-    <row r="657" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="657" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
         <v>1745</v>
       </c>
       <c r="B657" t="s">
-        <v>1855</v>
+        <v>1852</v>
       </c>
       <c r="C657" t="s">
-        <v>1856</v>
+        <v>1853</v>
       </c>
       <c r="D657" s="1" t="s">
-        <v>1857</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="658" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16405,13 +16414,13 @@
         <v>1745</v>
       </c>
       <c r="B658" t="s">
-        <v>1858</v>
+        <v>1855</v>
       </c>
       <c r="C658" t="s">
-        <v>1859</v>
+        <v>1856</v>
       </c>
       <c r="D658" s="1" t="s">
-        <v>1860</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="659" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16419,69 +16428,69 @@
         <v>1745</v>
       </c>
       <c r="B659" t="s">
-        <v>1861</v>
+        <v>1858</v>
       </c>
       <c r="C659" t="s">
-        <v>1862</v>
+        <v>1859</v>
       </c>
       <c r="D659" s="1" t="s">
-        <v>1863</v>
-      </c>
-    </row>
-    <row r="660" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="660" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A660" t="s">
         <v>1745</v>
       </c>
       <c r="B660" t="s">
-        <v>1864</v>
+        <v>1861</v>
       </c>
       <c r="C660" t="s">
-        <v>1865</v>
+        <v>1862</v>
       </c>
       <c r="D660" s="1" t="s">
-        <v>1866</v>
-      </c>
-    </row>
-    <row r="661" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="661" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
         <v>1745</v>
       </c>
       <c r="B661" t="s">
-        <v>78</v>
+        <v>1864</v>
       </c>
       <c r="C661" t="s">
-        <v>556</v>
+        <v>1865</v>
       </c>
       <c r="D661" s="1" t="s">
-        <v>1867</v>
-      </c>
-    </row>
-    <row r="662" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="662" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
         <v>1745</v>
       </c>
       <c r="B662" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C662" t="s">
-        <v>82</v>
+        <v>556</v>
       </c>
       <c r="D662" s="1" t="s">
-        <v>1868</v>
-      </c>
-    </row>
-    <row r="663" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="663" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
         <v>1745</v>
       </c>
       <c r="B663" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C663" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D663" s="1" t="s">
-        <v>86</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="664" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16489,13 +16498,13 @@
         <v>1745</v>
       </c>
       <c r="B664" t="s">
-        <v>1869</v>
+        <v>84</v>
       </c>
       <c r="C664" t="s">
-        <v>1870</v>
+        <v>85</v>
       </c>
       <c r="D664" s="1" t="s">
-        <v>1871</v>
+        <v>86</v>
       </c>
     </row>
     <row r="665" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16503,13 +16512,13 @@
         <v>1745</v>
       </c>
       <c r="B665" t="s">
-        <v>1872</v>
+        <v>1869</v>
       </c>
       <c r="C665" t="s">
-        <v>1873</v>
+        <v>1870</v>
       </c>
       <c r="D665" s="1" t="s">
-        <v>1874</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="666" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16517,13 +16526,13 @@
         <v>1745</v>
       </c>
       <c r="B666" t="s">
-        <v>1875</v>
+        <v>1872</v>
       </c>
       <c r="C666" t="s">
-        <v>1876</v>
+        <v>1873</v>
       </c>
       <c r="D666" s="1" t="s">
-        <v>1877</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="667" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16531,41 +16540,41 @@
         <v>1745</v>
       </c>
       <c r="B667" t="s">
-        <v>1878</v>
+        <v>1875</v>
       </c>
       <c r="C667" t="s">
-        <v>1879</v>
+        <v>1876</v>
       </c>
       <c r="D667" s="1" t="s">
-        <v>1880</v>
-      </c>
-    </row>
-    <row r="668" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="668" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A668" t="s">
         <v>1745</v>
       </c>
       <c r="B668" t="s">
-        <v>1881</v>
+        <v>1878</v>
       </c>
       <c r="C668" t="s">
-        <v>1882</v>
+        <v>1879</v>
       </c>
       <c r="D668" s="1" t="s">
-        <v>1883</v>
-      </c>
-    </row>
-    <row r="669" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="669" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A669" t="s">
         <v>1745</v>
       </c>
       <c r="B669" t="s">
-        <v>1884</v>
+        <v>1881</v>
       </c>
       <c r="C669" t="s">
-        <v>1885</v>
+        <v>1882</v>
       </c>
       <c r="D669" s="1" t="s">
-        <v>1886</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="670" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16573,13 +16582,13 @@
         <v>1745</v>
       </c>
       <c r="B670" t="s">
-        <v>1887</v>
+        <v>1884</v>
       </c>
       <c r="C670" t="s">
-        <v>1888</v>
+        <v>1885</v>
       </c>
       <c r="D670" s="1" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="671" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16587,13 +16596,13 @@
         <v>1745</v>
       </c>
       <c r="B671" t="s">
-        <v>1890</v>
+        <v>1887</v>
       </c>
       <c r="C671" t="s">
-        <v>1891</v>
+        <v>1888</v>
       </c>
       <c r="D671" s="1" t="s">
-        <v>1892</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="672" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16601,13 +16610,13 @@
         <v>1745</v>
       </c>
       <c r="B672" t="s">
-        <v>90</v>
+        <v>1890</v>
       </c>
       <c r="C672" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="D672" s="1" t="s">
-        <v>92</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="673" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16615,13 +16624,13 @@
         <v>1745</v>
       </c>
       <c r="B673" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C673" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="D673" s="1" t="s">
-        <v>1895</v>
+        <v>92</v>
       </c>
     </row>
     <row r="674" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16629,13 +16638,13 @@
         <v>1745</v>
       </c>
       <c r="B674" t="s">
-        <v>1896</v>
+        <v>93</v>
       </c>
       <c r="C674" t="s">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="D674" s="1" t="s">
-        <v>1898</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="675" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16643,13 +16652,13 @@
         <v>1745</v>
       </c>
       <c r="B675" t="s">
-        <v>96</v>
+        <v>1896</v>
       </c>
       <c r="C675" t="s">
-        <v>97</v>
+        <v>1897</v>
       </c>
       <c r="D675" s="1" t="s">
-        <v>98</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="676" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16657,13 +16666,13 @@
         <v>1745</v>
       </c>
       <c r="B676" t="s">
-        <v>1899</v>
+        <v>96</v>
       </c>
       <c r="C676" t="s">
-        <v>1900</v>
+        <v>97</v>
       </c>
       <c r="D676" s="1" t="s">
-        <v>1901</v>
+        <v>98</v>
       </c>
     </row>
     <row r="677" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16671,13 +16680,13 @@
         <v>1745</v>
       </c>
       <c r="B677" t="s">
-        <v>1902</v>
+        <v>1899</v>
       </c>
       <c r="C677" t="s">
-        <v>1903</v>
+        <v>1900</v>
       </c>
       <c r="D677" s="1" t="s">
-        <v>1904</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="678" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16685,13 +16694,13 @@
         <v>1745</v>
       </c>
       <c r="B678" t="s">
-        <v>1905</v>
+        <v>1902</v>
       </c>
       <c r="C678" t="s">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="D678" s="1" t="s">
-        <v>1907</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="679" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16699,13 +16708,13 @@
         <v>1745</v>
       </c>
       <c r="B679" t="s">
-        <v>1908</v>
+        <v>1905</v>
       </c>
       <c r="C679" t="s">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="D679" s="1" t="s">
-        <v>1910</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="680" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16713,13 +16722,13 @@
         <v>1745</v>
       </c>
       <c r="B680" t="s">
-        <v>1911</v>
+        <v>1908</v>
       </c>
       <c r="C680" t="s">
-        <v>1912</v>
+        <v>1909</v>
       </c>
       <c r="D680" s="1" t="s">
-        <v>1913</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="681" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16727,13 +16736,13 @@
         <v>1745</v>
       </c>
       <c r="B681" t="s">
-        <v>1914</v>
+        <v>1911</v>
       </c>
       <c r="C681" t="s">
-        <v>1915</v>
+        <v>1912</v>
       </c>
       <c r="D681" s="1" t="s">
-        <v>1916</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="682" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16741,13 +16750,13 @@
         <v>1745</v>
       </c>
       <c r="B682" t="s">
-        <v>1917</v>
+        <v>1914</v>
       </c>
       <c r="C682" t="s">
-        <v>1918</v>
+        <v>1915</v>
       </c>
       <c r="D682" s="1" t="s">
-        <v>1919</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="683" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16755,27 +16764,27 @@
         <v>1745</v>
       </c>
       <c r="B683" t="s">
-        <v>127</v>
+        <v>1917</v>
       </c>
       <c r="C683" t="s">
-        <v>128</v>
+        <v>1918</v>
       </c>
       <c r="D683" s="1" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="684" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A684" t="s">
-        <v>1921</v>
+        <v>1745</v>
       </c>
       <c r="B684" t="s">
-        <v>341</v>
+        <v>127</v>
       </c>
       <c r="C684" t="s">
-        <v>342</v>
+        <v>128</v>
       </c>
       <c r="D684" s="1" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="685" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16783,13 +16792,13 @@
         <v>1921</v>
       </c>
       <c r="B685" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C685" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D685" s="1" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="686" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16797,13 +16806,13 @@
         <v>1921</v>
       </c>
       <c r="B686" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C686" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D686" s="1" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="687" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16811,13 +16820,13 @@
         <v>1921</v>
       </c>
       <c r="B687" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C687" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D687" s="1" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="688" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16825,27 +16834,27 @@
         <v>1921</v>
       </c>
       <c r="B688" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C688" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D688" s="1" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="689" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A689" t="s">
-        <v>734</v>
+        <v>1921</v>
       </c>
       <c r="B689" t="s">
-        <v>735</v>
+        <v>353</v>
       </c>
       <c r="C689" t="s">
-        <v>736</v>
+        <v>354</v>
       </c>
       <c r="D689" s="1" t="s">
-        <v>737</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="690" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16853,13 +16862,13 @@
         <v>734</v>
       </c>
       <c r="B690" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="C690" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D690" s="1" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="691" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16867,13 +16876,13 @@
         <v>734</v>
       </c>
       <c r="B691" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="C691" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="D691" s="1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="692" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16881,12 +16890,26 @@
         <v>734</v>
       </c>
       <c r="B692" t="s">
+        <v>741</v>
+      </c>
+      <c r="C692" t="s">
+        <v>742</v>
+      </c>
+      <c r="D692" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="693" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A693" t="s">
+        <v>734</v>
+      </c>
+      <c r="B693" t="s">
         <v>744</v>
       </c>
-      <c r="C692" t="s">
+      <c r="C693" t="s">
         <v>745</v>
       </c>
-      <c r="D692" s="1" t="s">
+      <c r="D693" s="1" t="s">
         <v>746</v>
       </c>
     </row>

</xml_diff>